<commit_message>
This should be done
</commit_message>
<xml_diff>
--- a/csv-offers/offers.xlsx
+++ b/csv-offers/offers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\nodetess\csv-offers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1965EE1-BE0F-42ED-A0A0-BC421F444B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94078C24-39BF-45C8-BF58-83E957EE30B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4F9CA8C7-3413-B647-AEC2-4A186E5DA79A}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Telavox " sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="37">
-  <si>
-    <t xml:space="preserve">Forbrugsafregnet </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="35">
   <si>
     <t>3 timer &amp; 300 MB</t>
   </si>
@@ -109,9 +105,6 @@
   </si>
   <si>
     <t xml:space="preserve">DK-Lille </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basis </t>
   </si>
   <si>
     <t>MBB1</t>
@@ -512,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3224F52F-6B8A-C844-A8DE-3A034D903889}">
-  <dimension ref="A1:Q50"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O29" sqref="A29:O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -535,10 +528,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1">
         <v>0.3</v>
@@ -574,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -582,10 +575,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -621,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -629,10 +622,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -668,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -676,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>75</v>
@@ -715,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -723,28 +716,28 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>999</v>
+        <v>0.3</v>
       </c>
       <c r="E5">
-        <v>999</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>999</v>
+        <v>300</v>
       </c>
       <c r="G5">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -753,16 +746,16 @@
         <v>3</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N5" s="3">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -770,19 +763,19 @@
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="F6">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -800,16 +793,16 @@
         <v>3</v>
       </c>
       <c r="L6" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M6" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N6" s="3">
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -817,13 +810,13 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E7">
         <v>1000</v>
@@ -847,16 +840,16 @@
         <v>3</v>
       </c>
       <c r="L7" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="M7" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="N7" s="3">
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -864,13 +857,13 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E8">
         <v>1000</v>
@@ -894,36 +887,36 @@
         <v>3</v>
       </c>
       <c r="L8" s="3">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="M8" s="3">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="N8" s="3">
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>75</v>
+        <v>0.3</v>
       </c>
       <c r="E9">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -941,16 +934,16 @@
         <v>3</v>
       </c>
       <c r="L9" s="3">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="M9" s="3">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="N9" s="3">
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -958,28 +951,28 @@
         <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F10">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="G10">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -988,16 +981,16 @@
         <v>3</v>
       </c>
       <c r="L10" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M10" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N10" s="3">
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1005,19 +998,19 @@
         <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>0.3</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="F11">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1035,16 +1028,16 @@
         <v>3</v>
       </c>
       <c r="L11" s="3">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="M11" s="3">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="N11" s="3">
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1052,13 +1045,13 @@
         <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="E12">
         <v>1000</v>
@@ -1082,36 +1075,36 @@
         <v>3</v>
       </c>
       <c r="L12" s="3">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="M12" s="3">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="N12" s="3">
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>25</v>
+        <v>0.3</v>
       </c>
       <c r="E13">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1129,30 +1122,30 @@
         <v>3</v>
       </c>
       <c r="L13" s="3">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="M13" s="3">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="N13" s="3">
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>1000</v>
@@ -1176,16 +1169,16 @@
         <v>3</v>
       </c>
       <c r="L14" s="3">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="M14" s="3">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="N14" s="3">
         <v>0</v>
       </c>
       <c r="O14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1193,28 +1186,28 @@
         <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>999</v>
+        <v>25</v>
       </c>
       <c r="E15">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F15">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="G15">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1223,16 +1216,16 @@
         <v>3</v>
       </c>
       <c r="L15" s="3">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="M15" s="3">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="N15" s="3">
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1240,19 +1233,19 @@
         <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>0.3</v>
+        <v>75</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="F16">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1270,36 +1263,36 @@
         <v>3</v>
       </c>
       <c r="L16" s="3">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="M16" s="3">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="N16" s="3">
         <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="E17">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1317,30 +1310,30 @@
         <v>3</v>
       </c>
       <c r="L17" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M17" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="N17" s="3">
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>1000</v>
@@ -1364,30 +1357,30 @@
         <v>3</v>
       </c>
       <c r="L18" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="M18" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="N18" s="3">
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="E19">
         <v>1000</v>
@@ -1411,16 +1404,16 @@
         <v>3</v>
       </c>
       <c r="L19" s="3">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="M19" s="3">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="N19" s="3">
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -1428,28 +1421,28 @@
         <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>999</v>
+        <v>75</v>
       </c>
       <c r="E20">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F20">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="G20">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1458,27 +1451,30 @@
         <v>3</v>
       </c>
       <c r="L20" s="3">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="M20" s="3">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="N20" s="3">
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>0.3</v>
@@ -1514,18 +1510,18 @@
         <v>0</v>
       </c>
       <c r="O21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1561,18 +1557,18 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <v>25</v>
@@ -1608,18 +1604,18 @@
         <v>0</v>
       </c>
       <c r="O23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D24">
         <v>75</v>
@@ -1655,39 +1651,36 @@
         <v>0</v>
       </c>
       <c r="O24" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>999</v>
+        <v>0.3</v>
       </c>
       <c r="E25">
-        <v>999</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>999</v>
+        <v>300</v>
       </c>
       <c r="G25">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -1696,36 +1689,36 @@
         <v>3</v>
       </c>
       <c r="L25" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M25" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N25" s="3">
         <v>0</v>
       </c>
       <c r="O25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="F26">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1743,30 +1736,30 @@
         <v>3</v>
       </c>
       <c r="L26" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M26" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N26" s="3">
         <v>0</v>
       </c>
       <c r="O26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E27">
         <v>1000</v>
@@ -1790,30 +1783,30 @@
         <v>3</v>
       </c>
       <c r="L27" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="M27" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="N27" s="3">
         <v>0</v>
       </c>
       <c r="O27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
       <c r="D28">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E28">
         <v>1000</v>
@@ -1837,36 +1830,36 @@
         <v>3</v>
       </c>
       <c r="L28" s="3">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="M28" s="3">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="N28" s="3">
         <v>0</v>
       </c>
       <c r="O28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>75</v>
+        <v>0.3</v>
       </c>
       <c r="E29">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="F29">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1884,45 +1877,45 @@
         <v>3</v>
       </c>
       <c r="L29" s="3">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="M29" s="3">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="N29" s="3">
         <v>0</v>
       </c>
       <c r="O29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F30">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="G30">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="H30">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -1931,36 +1924,36 @@
         <v>3</v>
       </c>
       <c r="L30" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M30" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N30" s="3">
         <v>0</v>
       </c>
       <c r="O30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>0.3</v>
+        <v>25</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="F31">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1978,30 +1971,30 @@
         <v>3</v>
       </c>
       <c r="L31" s="3">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="M31" s="3">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="N31" s="3">
         <v>0</v>
       </c>
       <c r="O31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="E32">
         <v>1000</v>
@@ -2025,42 +2018,42 @@
         <v>3</v>
       </c>
       <c r="L32" s="3">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="M32" s="3">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="N32" s="3">
         <v>0</v>
       </c>
       <c r="O32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>70</v>
-      </c>
-      <c r="B33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C33" t="s">
-        <v>3</v>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D33">
-        <v>25</v>
+        <v>0.5</v>
       </c>
       <c r="E33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -2072,42 +2065,42 @@
         <v>3</v>
       </c>
       <c r="L33" s="3">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="M33" s="3">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="N33" s="3">
         <v>0</v>
       </c>
       <c r="O33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>70</v>
-      </c>
-      <c r="B34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C34" t="s">
-        <v>4</v>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D34">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -2119,45 +2112,45 @@
         <v>3</v>
       </c>
       <c r="L34" s="3">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="M34" s="3">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="N34" s="3">
         <v>0</v>
       </c>
       <c r="O34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C35" t="s">
-        <v>0</v>
+      <c r="C35" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D35">
-        <v>999</v>
+        <v>50</v>
       </c>
       <c r="E35">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>999</v>
       </c>
       <c r="G35">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -2166,45 +2159,45 @@
         <v>3</v>
       </c>
       <c r="L35" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="M35" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N35" s="3">
         <v>0</v>
       </c>
       <c r="O35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -2213,45 +2206,45 @@
         <v>3</v>
       </c>
       <c r="L36" s="3">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="M36" s="3">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="N36" s="3">
         <v>0</v>
       </c>
       <c r="O36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>0</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -2260,45 +2253,45 @@
         <v>3</v>
       </c>
       <c r="L37" s="3">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="M37" s="3">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N37" s="3">
         <v>0</v>
       </c>
       <c r="O37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -2307,45 +2300,45 @@
         <v>3</v>
       </c>
       <c r="L38" s="3">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="M38" s="3">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="N38" s="3">
         <v>0</v>
       </c>
       <c r="O38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>0</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
-        <v>4</v>
+        <v>40</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -2354,45 +2347,45 @@
         <v>3</v>
       </c>
       <c r="L39" s="3">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="M39" s="3">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="N39" s="3">
         <v>0</v>
       </c>
       <c r="O39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
         <v>999</v>
       </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
       <c r="H40">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -2401,45 +2394,45 @@
         <v>3</v>
       </c>
       <c r="L40" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="M40" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N40" s="3">
         <v>0</v>
       </c>
       <c r="O40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
         <v>999</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
       <c r="H41">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -2448,45 +2441,45 @@
         <v>3</v>
       </c>
       <c r="L41" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="M41" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="N41" s="3">
         <v>0</v>
       </c>
       <c r="O41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
       <c r="D42">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
         <v>999</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
       <c r="H42">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -2495,24 +2488,24 @@
         <v>3</v>
       </c>
       <c r="L42" s="3">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="M42" s="3">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="N42" s="3">
         <v>0</v>
       </c>
       <c r="O42" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2542,345 +2535,16 @@
         <v>3</v>
       </c>
       <c r="L43" s="3">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="M43" s="3">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="N43" s="3">
         <v>0</v>
       </c>
       <c r="O43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>20</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>999</v>
-      </c>
-      <c r="H44">
-        <v>999</v>
-      </c>
-      <c r="I44">
-        <v>999</v>
-      </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44">
-        <v>3</v>
-      </c>
-      <c r="L44" s="3">
-        <v>60</v>
-      </c>
-      <c r="M44" s="3">
-        <v>60</v>
-      </c>
-      <c r="N44" s="3">
-        <v>0</v>
-      </c>
-      <c r="O44" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>30</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>999</v>
-      </c>
-      <c r="H45">
-        <v>999</v>
-      </c>
-      <c r="I45">
-        <v>999</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>3</v>
-      </c>
-      <c r="L45" s="3">
-        <v>50</v>
-      </c>
-      <c r="M45" s="3">
-        <v>50</v>
-      </c>
-      <c r="N45" s="3">
-        <v>0</v>
-      </c>
-      <c r="O45" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>40</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>999</v>
-      </c>
-      <c r="H46">
-        <v>999</v>
-      </c>
-      <c r="I46">
-        <v>999</v>
-      </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-      <c r="K46">
-        <v>3</v>
-      </c>
-      <c r="L46" s="3">
-        <v>40</v>
-      </c>
-      <c r="M46" s="3">
-        <v>40</v>
-      </c>
-      <c r="N46" s="3">
-        <v>0</v>
-      </c>
-      <c r="O46" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>50</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>999</v>
-      </c>
-      <c r="H47">
-        <v>999</v>
-      </c>
-      <c r="I47">
-        <v>999</v>
-      </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <v>3</v>
-      </c>
-      <c r="L47" s="3">
-        <v>30</v>
-      </c>
-      <c r="M47" s="3">
-        <v>30</v>
-      </c>
-      <c r="N47" s="3">
-        <v>0</v>
-      </c>
-      <c r="O47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>60</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>999</v>
-      </c>
-      <c r="H48">
-        <v>999</v>
-      </c>
-      <c r="I48">
-        <v>999</v>
-      </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
-        <v>3</v>
-      </c>
-      <c r="L48" s="3">
-        <v>20</v>
-      </c>
-      <c r="M48" s="3">
-        <v>20</v>
-      </c>
-      <c r="N48" s="3">
-        <v>0</v>
-      </c>
-      <c r="O48" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>70</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <v>999</v>
-      </c>
-      <c r="H49">
-        <v>999</v>
-      </c>
-      <c r="I49">
-        <v>999</v>
-      </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
-      <c r="K49">
-        <v>3</v>
-      </c>
-      <c r="L49" s="3">
-        <v>10</v>
-      </c>
-      <c r="M49" s="3">
-        <v>10</v>
-      </c>
-      <c r="N49" s="3">
-        <v>0</v>
-      </c>
-      <c r="O49" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>0</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>999</v>
-      </c>
-      <c r="H50">
-        <v>999</v>
-      </c>
-      <c r="I50">
-        <v>999</v>
-      </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <v>3</v>
-      </c>
-      <c r="L50" s="3">
-        <v>5</v>
-      </c>
-      <c r="M50" s="3">
-        <v>5</v>
-      </c>
-      <c r="N50" s="3">
-        <v>0</v>
-      </c>
-      <c r="O50" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2890,10 +2554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC21A78-6651-514A-AC8A-9FD0233948C2}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="O7" sqref="A7:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2911,10 +2575,10 @@
         <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1">
         <v>30</v>
@@ -2950,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="O1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -2958,10 +2622,10 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>30</v>
@@ -2997,7 +2661,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -3005,10 +2669,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3044,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -3052,10 +2716,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>0.5</v>
@@ -3091,7 +2755,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3099,10 +2763,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -3138,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -3146,10 +2810,10 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3185,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -3196,25 +2860,25 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>999</v>
       </c>
       <c r="G7">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -3223,16 +2887,16 @@
         <v>3</v>
       </c>
       <c r="L7">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="M7">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -3240,13 +2904,13 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3270,16 +2934,16 @@
         <v>3</v>
       </c>
       <c r="L8">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="M8">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -3287,13 +2951,13 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -3317,16 +2981,16 @@
         <v>3</v>
       </c>
       <c r="L9">
-        <v>89</v>
+        <v>144</v>
       </c>
       <c r="M9">
-        <v>89</v>
+        <v>144</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -3334,13 +2998,13 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -3364,16 +3028,16 @@
         <v>3</v>
       </c>
       <c r="L10">
-        <v>144</v>
+        <v>209</v>
       </c>
       <c r="M10">
-        <v>144</v>
+        <v>209</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -3381,13 +3045,13 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3411,16 +3075,16 @@
         <v>3</v>
       </c>
       <c r="L11">
-        <v>209</v>
+        <v>269</v>
       </c>
       <c r="M11">
-        <v>209</v>
+        <v>269</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -3428,13 +3092,13 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>75</v>
+        <v>200</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3458,45 +3122,45 @@
         <v>3</v>
       </c>
       <c r="L12">
-        <v>269</v>
+        <v>349</v>
       </c>
       <c r="M12">
-        <v>269</v>
+        <v>349</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D13">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
         <v>999</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
       <c r="H13">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -3505,27 +3169,28 @@
         <v>3</v>
       </c>
       <c r="L13">
-        <v>349</v>
+        <f>5+15+50</f>
+        <v>70</v>
       </c>
       <c r="M13">
-        <v>349</v>
+        <v>70</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="O13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -3559,10 +3224,10 @@
         <v>70</v>
       </c>
       <c r="N14">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="O14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3570,28 +3235,28 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -3600,77 +3265,76 @@
         <v>3</v>
       </c>
       <c r="L15">
-        <f>5+15+50</f>
-        <v>70</v>
+        <f>50+60</f>
+        <v>110</v>
       </c>
       <c r="M15">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="N15">
-        <v>65</v>
+        <f>(4*75)+350</f>
+        <v>650</v>
       </c>
       <c r="O15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>59</v>
+      </c>
+      <c r="M16">
+        <v>59</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
         <v>33</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>3</v>
-      </c>
-      <c r="L16">
-        <f>50+60</f>
-        <v>110</v>
-      </c>
-      <c r="M16">
-        <v>110</v>
-      </c>
-      <c r="N16">
-        <f>(4*75)+350</f>
-        <v>650</v>
-      </c>
-      <c r="O16" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -3697,27 +3361,27 @@
         <v>3</v>
       </c>
       <c r="L17">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="M17">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="N17">
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3744,27 +3408,27 @@
         <v>3</v>
       </c>
       <c r="L18">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="M18">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -3791,63 +3455,16 @@
         <v>3</v>
       </c>
       <c r="L19">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="M19">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>3</v>
-      </c>
-      <c r="L20">
-        <v>19</v>
-      </c>
-      <c r="M20">
-        <v>19</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3879,10 +3496,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1">
         <v>1</v>
@@ -3918,7 +3535,7 @@
         <v>0</v>
       </c>
       <c r="O1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -3926,10 +3543,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -3967,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -3975,10 +3592,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -4016,7 +3633,7 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -4024,10 +3641,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -4065,7 +3682,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -4073,10 +3690,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -4114,7 +3731,7 @@
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -4122,10 +3739,10 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>100</v>
@@ -4163,7 +3780,7 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -4171,10 +3788,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -4212,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -4220,10 +3837,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -4261,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -4269,10 +3886,10 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -4310,7 +3927,7 @@
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -4318,10 +3935,10 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>25</v>
@@ -4359,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -4367,10 +3984,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -4408,7 +4025,7 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -4416,10 +4033,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>100</v>
@@ -4457,7 +4074,7 @@
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -4465,10 +4082,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -4504,7 +4121,7 @@
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -4512,10 +4129,10 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -4553,7 +4170,7 @@
         <v>0</v>
       </c>
       <c r="O14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -4561,10 +4178,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -4600,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -4608,10 +4225,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -4647,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -4655,10 +4272,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -4694,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -4702,10 +4319,10 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18">
         <v>25</v>
@@ -4741,7 +4358,7 @@
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -4749,10 +4366,10 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19">
         <v>50</v>
@@ -4788,7 +4405,7 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -4796,10 +4413,10 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -4835,7 +4452,7 @@
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -4843,10 +4460,10 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -4882,7 +4499,7 @@
         <v>0</v>
       </c>
       <c r="O21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -4890,10 +4507,10 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -4929,7 +4546,7 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>